<commit_message>
Rename variables and update dictionary
</commit_message>
<xml_diff>
--- a/data-raw/dictionary.xlsx
+++ b/data-raw/dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sloos\Documents\git-repositories\cbssuitabilityhaiti\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C0C660-225B-4F2C-9101-C02011FBBB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E813FFD4-36A4-4D98-9EFF-4CCBD92B277C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20295" yWindow="1725" windowWidth="17250" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1170" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
   <si>
     <t>directory</t>
   </si>
@@ -58,9 +58,6 @@
     <t>sup_km2</t>
   </si>
   <si>
-    <t>sector_id</t>
-  </si>
-  <si>
     <t>cte</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
     <t>density</t>
   </si>
   <si>
+    <t>integer</t>
+  </si>
+  <si>
     <t>aptitude</t>
   </si>
   <si>
@@ -118,22 +118,67 @@
     <t>mwater.rda</t>
   </si>
   <si>
-    <t>Latitude.o</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Administra</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Date.added</t>
-  </si>
-  <si>
-    <t>Datasets..</t>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>administra</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>date_added</t>
+  </si>
+  <si>
+    <t>datasets</t>
+  </si>
+  <si>
+    <t>Unique identifying number for each neighborhood unit</t>
+  </si>
+  <si>
+    <t>Name of each nieghborhood unit</t>
+  </si>
+  <si>
+    <t>Area of neighborhood in square km</t>
+  </si>
+  <si>
+    <t>Name of commune (administrative unit in Haiti)</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Categorical socioeconomic status (low, medium)</t>
+  </si>
+  <si>
+    <t>area of neihborhood covered by buildings in square meters</t>
+  </si>
+  <si>
+    <t>Categorical population density (least dense, somewhat dense, dense, very dense, most dense)</t>
+  </si>
+  <si>
+    <t>suitability of the site for a wastewater treatment system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"group" if collective or grouped sanitation is possible in short term. </t>
+  </si>
+  <si>
+    <t>Suggested pit latrine and septic allowance (allowed, not allowed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown </t>
+  </si>
+  <si>
+    <t>Catgoriccal population density according to the description of the variable "density" (values from 1 to 5)</t>
+  </si>
+  <si>
+    <t>Categotical socioeconomic status according to the description of the variable "economy" (1=low, 2 = medium)</t>
+  </si>
+  <si>
+    <t>Geospatial data of the neighborhood stored as a polygon</t>
   </si>
   <si>
     <t>Lattitude coordinate</t>
@@ -152,54 +197,6 @@
   </si>
   <si>
     <t>Dataset in mWater that point is part of, including organizaiton that is responsible for data</t>
-  </si>
-  <si>
-    <t>Unique identifying number for each neighborhood unit</t>
-  </si>
-  <si>
-    <t>Name of each nieghborhood unit</t>
-  </si>
-  <si>
-    <t>Area of neighborhood in square km</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Name of commune (administrative unit in Haiti)</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>Categorical socioeconomic status (low, medium)</t>
-  </si>
-  <si>
-    <t>Categorical population density (least dense, somewhat dense, dense, very dense, most dense)</t>
-  </si>
-  <si>
-    <t>Suggested pit latrine and septic allowance (allowed, not allowed)</t>
-  </si>
-  <si>
-    <t>area of neihborhood covered by buildings in square meters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"group" if collective or grouped sanitation is possible in short term. </t>
-  </si>
-  <si>
-    <t>suitability of the site for a wastewater treatment system</t>
-  </si>
-  <si>
-    <t>Catgoriccal population density according to the description of the variable "density" (values from 1 to 5)</t>
-  </si>
-  <si>
-    <t>Categotical socioeconomic status according to the description of the variable "economy" (1=low, 2 = medium)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown </t>
-  </si>
-  <si>
-    <t>Geospatial data of the neighborhood stored as a polygon</t>
   </si>
   <si>
     <t>Geospatial data of the different access points that were added to mWater</t>
@@ -536,13 +533,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="97.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -575,7 +575,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -592,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -609,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -623,10 +623,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -640,10 +640,10 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -677,7 +677,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -694,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -725,10 +725,10 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -742,10 +742,10 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -776,10 +776,10 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -790,13 +790,13 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -807,13 +807,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -824,13 +824,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -841,13 +841,13 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -858,13 +858,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -875,13 +875,13 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -892,13 +892,13 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -906,16 +906,16 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -926,13 +926,13 @@
         <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -943,13 +943,13 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -960,13 +960,13 @@
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -977,13 +977,13 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -994,13 +994,13 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1011,30 +1011,13 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change variable sup_bati to sup_bati_km2
</commit_message>
<xml_diff>
--- a/data-raw/dictionary.xlsx
+++ b/data-raw/dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sloos\Documents\git-repositories\cbssuitabilityhaiti\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E813FFD4-36A4-4D98-9EFF-4CCBD92B277C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982281DC-7289-42EA-BD4C-4CDCF5F1D6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1170" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5736" yWindow="0" windowWidth="17304" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>ranking</t>
   </si>
   <si>
-    <t>sup_bati</t>
-  </si>
-  <si>
     <t>density</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>Categorical socioeconomic status (low, medium)</t>
   </si>
   <si>
-    <t>area of neihborhood covered by buildings in square meters</t>
-  </si>
-  <si>
     <t>Categorical population density (least dense, somewhat dense, dense, very dense, most dense)</t>
   </si>
   <si>
@@ -200,6 +194,12 @@
   </si>
   <si>
     <t>Geospatial data of the different access points that were added to mWater</t>
+  </si>
+  <si>
+    <t>sup_bati_km2</t>
+  </si>
+  <si>
+    <t>area of neihborhood covered by buildings in square kilometers</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,7 +575,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -592,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -609,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -626,7 +626,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -660,7 +660,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -677,7 +677,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -694,7 +694,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -728,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -745,7 +745,7 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -756,13 +756,13 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -773,13 +773,13 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -790,13 +790,13 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -807,13 +807,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -824,13 +824,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -841,13 +841,13 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -858,13 +858,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -875,13 +875,13 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -892,13 +892,13 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="D21" t="s">
-        <v>30</v>
-      </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -906,16 +906,16 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
       <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -923,16 +923,16 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -940,16 +940,16 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -957,16 +957,16 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -974,16 +974,16 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -991,16 +991,16 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1008,16 +1008,16 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
         <v>29</v>
       </c>
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>